<commit_message>
Update script for data analysis
</commit_message>
<xml_diff>
--- a/RP3 stim response, amp, 10-25.xlsx
+++ b/RP3 stim response, amp, 10-25.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apiskadlo/Documents/All Work/U of U/2023 School/Fall 2023/Brain/Labs/Research project 1/ResearchExperience1/mjhaptix/NENR_Project3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NENR_Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D100B6AC-52B4-994E-8380-BB922BBCD499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97501A86-31A2-4054-B8EA-959818169DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B53F8DC4-0488-B543-B87C-CD45CFC5D894}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B53F8DC4-0488-B543-B87C-CD45CFC5D894}"/>
   </bookViews>
   <sheets>
     <sheet name="Andrew" sheetId="1" r:id="rId1"/>
     <sheet name="AndrewV2" sheetId="4" r:id="rId2"/>
-    <sheet name="Wilson" sheetId="2" r:id="rId3"/>
-    <sheet name="Miru" sheetId="3" r:id="rId4"/>
+    <sheet name="Miru" sheetId="3" r:id="rId3"/>
+    <sheet name="Wilson" sheetId="2" r:id="rId4"/>
+    <sheet name="CombineData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="38">
   <si>
     <t>Particpant</t>
   </si>
@@ -138,13 +139,28 @@
   </si>
   <si>
     <t>1to 5</t>
+  </si>
+  <si>
+    <t>perceived intensity</t>
+  </si>
+  <si>
+    <t>Participant 1</t>
+  </si>
+  <si>
+    <t>Participant 2</t>
+  </si>
+  <si>
+    <t>Participant 3</t>
+  </si>
+  <si>
+    <t>Pulse Frequency (Hz)):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,13 +175,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,9 +208,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,24 +533,24 @@
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="7" max="9" width="25.875" customWidth="1"/>
+    <col min="10" max="10" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -531,7 +564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -575,7 +608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -613,7 +646,7 @@
         <v>270.66000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
@@ -645,7 +678,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
@@ -677,7 +710,7 @@
         <v>269.03500000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
@@ -709,7 +742,7 @@
         <v>266.72000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
@@ -738,7 +771,7 @@
         <v>6678.54</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
@@ -767,7 +800,7 @@
         <v>724.40800000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
@@ -796,7 +829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>8</v>
       </c>
@@ -813,112 +846,112 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>30</v>
       </c>
@@ -932,16 +965,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D07154-447C-BD47-AF54-C2AE88A7FE94}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="9" width="18.33203125" customWidth="1"/>
+    <col min="4" max="9" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -958,7 +991,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -975,7 +1008,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -994,7 +1027,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1052,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1064,7 +1097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E6">
         <v>40</v>
@@ -1103,14 +1136,14 @@
         <v>270.66000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -1138,14 +1171,14 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E8">
         <v>150</v>
@@ -1173,14 +1206,14 @@
         <v>269.03500000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E9">
         <v>200</v>
@@ -1208,14 +1241,14 @@
         <v>266.72000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
         <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E10">
         <v>250</v>
@@ -1241,14 +1274,14 @@
         <v>6678.54</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>6</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E11">
         <v>200</v>
@@ -1256,7 +1289,7 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>2</v>
       </c>
       <c r="H11" s="1"/>
@@ -1274,14 +1307,14 @@
         <v>724.40800000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>7</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E12">
         <v>200</v>
@@ -1289,7 +1322,7 @@
       <c r="F12">
         <v>60</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>3</v>
       </c>
       <c r="H12" s="1"/>
@@ -1307,14 +1340,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>8</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E13">
         <v>200</v>
@@ -1322,7 +1355,7 @@
       <c r="F13">
         <v>90</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>4</v>
       </c>
       <c r="H13" s="1"/>
@@ -1334,14 +1367,14 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <v>9</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E14">
         <v>200</v>
@@ -1349,7 +1382,7 @@
       <c r="F14">
         <v>120</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
         <v>4</v>
       </c>
       <c r="H14" s="1"/>
@@ -1361,14 +1394,14 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E15">
         <v>200</v>
@@ -1376,7 +1409,7 @@
       <c r="F15">
         <v>150</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
         <v>3</v>
       </c>
       <c r="H15" s="1"/>
@@ -1388,14 +1421,14 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>11</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E16">
         <v>200</v>
@@ -1403,7 +1436,7 @@
       <c r="F16">
         <v>180</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
         <v>5</v>
       </c>
       <c r="H16" s="1"/>
@@ -1415,14 +1448,14 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>12</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E17">
         <v>200</v>
@@ -1430,7 +1463,7 @@
       <c r="F17">
         <v>210</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="3">
         <v>5</v>
       </c>
       <c r="H17" s="1"/>
@@ -1442,14 +1475,14 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
         <v>13</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E18">
         <v>200</v>
@@ -1457,7 +1490,7 @@
       <c r="F18">
         <v>240</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
         <v>5</v>
       </c>
       <c r="H18" s="1"/>
@@ -1469,7 +1502,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
@@ -1488,7 +1521,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -1507,7 +1540,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -1526,7 +1559,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -1545,7 +1578,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
@@ -1564,7 +1597,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
@@ -1583,7 +1616,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -1602,7 +1635,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
@@ -1621,7 +1654,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
@@ -1640,7 +1673,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
@@ -1659,7 +1692,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
@@ -1678,7 +1711,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1">
@@ -1697,7 +1730,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1">
@@ -1716,7 +1749,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1">
@@ -1735,7 +1768,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1">
@@ -1754,7 +1787,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
@@ -1773,7 +1806,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1">
@@ -1798,24 +1831,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F16C671-261E-C941-BEA8-8AF7FC3D64A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AC17BD-CF39-1A46-9B0D-CC46562E2306}">
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F18"/>
+      <selection activeCell="G11" sqref="G11:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="15" width="18.83203125" customWidth="1"/>
+    <col min="4" max="15" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1829,7 +1862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1873,7 +1906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1884,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>40</v>
@@ -1902,12 +1935,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -1916,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
         <v>13</v>
@@ -1925,12 +1958,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>150</v>
@@ -1948,12 +1981,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>200</v>
@@ -1962,7 +1995,7 @@
         <v>30</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
@@ -1971,12 +2004,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>250</v>
@@ -1985,7 +2018,7 @@
         <v>30</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
         <v>13</v>
@@ -1994,12 +2027,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>200</v>
@@ -2007,7 +2040,7 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>2</v>
       </c>
       <c r="J11" t="s">
@@ -2017,12 +2050,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>200</v>
@@ -2030,8 +2063,8 @@
       <c r="F12">
         <v>60</v>
       </c>
-      <c r="G12">
-        <v>1</v>
+      <c r="G12" s="2">
+        <v>2</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
@@ -2040,12 +2073,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>8</v>
       </c>
       <c r="D13">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>200</v>
@@ -2053,8 +2086,8 @@
       <c r="F13">
         <v>90</v>
       </c>
-      <c r="G13">
-        <v>1</v>
+      <c r="G13" s="2">
+        <v>3</v>
       </c>
       <c r="J13" t="s">
         <v>13</v>
@@ -2063,12 +2096,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>200</v>
@@ -2076,8 +2109,8 @@
       <c r="F14">
         <v>120</v>
       </c>
-      <c r="G14">
-        <v>1</v>
+      <c r="G14" s="2">
+        <v>3</v>
       </c>
       <c r="J14" t="s">
         <v>13</v>
@@ -2086,12 +2119,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>200</v>
@@ -2099,8 +2132,8 @@
       <c r="F15">
         <v>150</v>
       </c>
-      <c r="G15">
-        <v>2</v>
+      <c r="G15" s="2">
+        <v>3</v>
       </c>
       <c r="J15" t="s">
         <v>13</v>
@@ -2109,12 +2142,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>11</v>
       </c>
       <c r="D16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>200</v>
@@ -2122,8 +2155,8 @@
       <c r="F16">
         <v>180</v>
       </c>
-      <c r="G16">
-        <v>2</v>
+      <c r="G16" s="2">
+        <v>3</v>
       </c>
       <c r="J16" t="s">
         <v>13</v>
@@ -2132,12 +2165,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>12</v>
       </c>
       <c r="D17">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>200</v>
@@ -2145,8 +2178,8 @@
       <c r="F17">
         <v>210</v>
       </c>
-      <c r="G17">
-        <v>2</v>
+      <c r="G17" s="2">
+        <v>4</v>
       </c>
       <c r="J17" t="s">
         <v>13</v>
@@ -2155,12 +2188,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>13</v>
       </c>
       <c r="D18">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>200</v>
@@ -2168,8 +2201,8 @@
       <c r="F18">
         <v>240</v>
       </c>
-      <c r="G18">
-        <v>1</v>
+      <c r="G18" s="2">
+        <v>3</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
@@ -2178,7 +2211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>14</v>
       </c>
@@ -2192,7 +2225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>15</v>
       </c>
@@ -2200,7 +2233,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>16</v>
       </c>
@@ -2208,7 +2241,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>17</v>
       </c>
@@ -2216,7 +2249,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>18</v>
       </c>
@@ -2224,7 +2257,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>19</v>
       </c>
@@ -2232,7 +2265,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>20</v>
       </c>
@@ -2240,7 +2273,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>21</v>
       </c>
@@ -2248,7 +2281,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>22</v>
       </c>
@@ -2256,7 +2289,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>23</v>
       </c>
@@ -2264,7 +2297,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>24</v>
       </c>
@@ -2272,7 +2305,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>25</v>
       </c>
@@ -2280,7 +2313,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>26</v>
       </c>
@@ -2288,7 +2321,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>27</v>
       </c>
@@ -2296,7 +2329,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>28</v>
       </c>
@@ -2304,7 +2337,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>29</v>
       </c>
@@ -2312,7 +2345,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>30</v>
       </c>
@@ -2326,24 +2359,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AC17BD-CF39-1A46-9B0D-CC46562E2306}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F16C671-261E-C941-BEA8-8AF7FC3D64A4}">
   <dimension ref="A3:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G11" sqref="G11:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="15" width="18.83203125" customWidth="1"/>
+    <col min="4" max="15" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2357,7 +2390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2401,7 +2434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2412,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E6">
         <v>40</v>
@@ -2430,12 +2463,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -2444,7 +2477,7 @@
         <v>30</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" t="s">
         <v>13</v>
@@ -2453,12 +2486,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E8">
         <v>150</v>
@@ -2476,12 +2509,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E9">
         <v>200</v>
@@ -2490,7 +2523,7 @@
         <v>30</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
@@ -2499,12 +2532,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E10">
         <v>250</v>
@@ -2513,7 +2546,7 @@
         <v>30</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
         <v>13</v>
@@ -2522,12 +2555,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E11">
         <v>200</v>
@@ -2535,7 +2568,7 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>2</v>
       </c>
       <c r="J11" t="s">
@@ -2545,12 +2578,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E12">
         <v>200</v>
@@ -2558,8 +2591,8 @@
       <c r="F12">
         <v>60</v>
       </c>
-      <c r="G12">
-        <v>2</v>
+      <c r="G12" s="2">
+        <v>1</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
@@ -2568,12 +2601,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>8</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E13">
         <v>200</v>
@@ -2581,8 +2614,8 @@
       <c r="F13">
         <v>90</v>
       </c>
-      <c r="G13">
-        <v>3</v>
+      <c r="G13" s="2">
+        <v>1</v>
       </c>
       <c r="J13" t="s">
         <v>13</v>
@@ -2591,12 +2624,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E14">
         <v>200</v>
@@ -2604,8 +2637,8 @@
       <c r="F14">
         <v>120</v>
       </c>
-      <c r="G14">
-        <v>3</v>
+      <c r="G14" s="2">
+        <v>1</v>
       </c>
       <c r="J14" t="s">
         <v>13</v>
@@ -2614,12 +2647,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E15">
         <v>200</v>
@@ -2627,8 +2660,8 @@
       <c r="F15">
         <v>150</v>
       </c>
-      <c r="G15">
-        <v>3</v>
+      <c r="G15" s="2">
+        <v>2</v>
       </c>
       <c r="J15" t="s">
         <v>13</v>
@@ -2637,12 +2670,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>11</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E16">
         <v>200</v>
@@ -2650,8 +2683,8 @@
       <c r="F16">
         <v>180</v>
       </c>
-      <c r="G16">
-        <v>3</v>
+      <c r="G16" s="2">
+        <v>2</v>
       </c>
       <c r="J16" t="s">
         <v>13</v>
@@ -2660,12 +2693,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>12</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E17">
         <v>200</v>
@@ -2673,8 +2706,8 @@
       <c r="F17">
         <v>210</v>
       </c>
-      <c r="G17">
-        <v>4</v>
+      <c r="G17" s="2">
+        <v>2</v>
       </c>
       <c r="J17" t="s">
         <v>13</v>
@@ -2683,12 +2716,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>13</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E18">
         <v>200</v>
@@ -2696,8 +2729,8 @@
       <c r="F18">
         <v>240</v>
       </c>
-      <c r="G18">
-        <v>3</v>
+      <c r="G18" s="2">
+        <v>1</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
@@ -2706,7 +2739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>14</v>
       </c>
@@ -2720,7 +2753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>15</v>
       </c>
@@ -2728,7 +2761,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>16</v>
       </c>
@@ -2736,7 +2769,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>17</v>
       </c>
@@ -2744,7 +2777,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>18</v>
       </c>
@@ -2752,7 +2785,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>19</v>
       </c>
@@ -2760,7 +2793,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>20</v>
       </c>
@@ -2768,7 +2801,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>21</v>
       </c>
@@ -2776,7 +2809,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>22</v>
       </c>
@@ -2784,7 +2817,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>23</v>
       </c>
@@ -2792,7 +2825,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>24</v>
       </c>
@@ -2800,7 +2833,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>25</v>
       </c>
@@ -2808,7 +2841,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>26</v>
       </c>
@@ -2816,7 +2849,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>27</v>
       </c>
@@ -2824,7 +2857,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>28</v>
       </c>
@@ -2832,7 +2865,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>29</v>
       </c>
@@ -2840,7 +2873,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>30</v>
       </c>
@@ -2851,4 +2884,253 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5F1538-F273-4BEE-9013-9EEB4748AF2E}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>200</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>250</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>90</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>180</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>210</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>240</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>